<commit_message>
Added output of results to XLSX file.
</commit_message>
<xml_diff>
--- a/AdapQuestBackend/data/templates/adaptive.results.template.xlsx
+++ b/AdapQuestBackend/data/templates/adaptive.results.template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\adaptive\adapquest\AdapQuestExperiments\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\adaptive\adapquest\AdapQuestBackend\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A298134-84CE-49C1-B273-E8E6B088DE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9C376B-2370-4158-AB17-CEDB00183361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4B693A07-E7FD-446E-A9F1-08BA55D2E17D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4B693A07-E7FD-446E-A9F1-08BA55D2E17D}"/>
   </bookViews>
   <sheets>
     <sheet name="results" sheetId="9" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>All Qs are only-yes</t>
+    <t>Observed skills</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3185,7 +3185,7 @@
       <selection pane="bottomRight" activeCell="A155" sqref="A155:XFD155"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
-      <autoFilter ref="A1:V919" xr:uid="{798640A0-EF78-4BAD-B3F6-C7172D43C7A6}">
+      <autoFilter ref="A1:V919" xr:uid="{54E39607-1F4B-4282-9EB8-C6306A291902}">
         <filterColumn colId="1">
           <customFilters>
             <customFilter operator="notEqual" val=" "/>

</xml_diff>